<commit_message>
Updated poc per school by level
</commit_message>
<xml_diff>
--- a/dps_dashboard/data/2021/school_stats_data/HS_poc_per_school_22.xlsx
+++ b/dps_dashboard/data/2021/school_stats_data/HS_poc_per_school_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melaniemoseley/CodingWorkspace/visualizing_DPS/dps_dashboard/data/2021/school_stats_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC3E4064-B2FA-E344-9312-E1EF75FF207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89E13FBF-379E-B246-B4F6-4A22B9E8A9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15640" xr2:uid="{8A77730F-63B3-7A4A-B171-15DB83AB20AC}"/>
   </bookViews>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF3A71A-D00B-3947-98E9-2D290A6041D4}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,80 +488,64 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
+      <c r="D12" s="4"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
+      <c r="D13" s="5"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
       <c r="D18" s="4"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D19" s="4"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="4"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="D21" s="5"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C27" s="3"/>
-      <c r="D27" s="5"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>